<commit_message>
Cart clean code added
</commit_message>
<xml_diff>
--- a/ExcelSheet/Order ID Creation Test Data.xlsx
+++ b/ExcelSheet/Order ID Creation Test Data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thangapandiyan P\eclipse-workspace\Grocery\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE583892-FA43-4273-AFD7-C961EEB14A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE63C4EE-C189-41CE-B81D-CCCDBA4D809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B0FA13CD-A657-4B1F-BFBF-A9EC59F170FD}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -111,19 +111,32 @@
     <t>5555555555552222</t>
   </si>
   <si>
-    <t>904916</t>
+    <t>165585</t>
   </si>
   <si>
     <t>Happilo 100% Natural Premium California Almonds | Premium Badam Giri</t>
   </si>
   <si>
     <t>$580.00</t>
+  </si>
+  <si>
+    <t>477909</t>
+  </si>
+  <si>
+    <t>$1200.00</t>
+  </si>
+  <si>
+    <t>201310</t>
+  </si>
+  <si>
+    <t>$1650.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -488,26 +501,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC29B1E-7B10-4AEB-96D6-BAB5E69ADB9B}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.59765625" customWidth="1"/>
-    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.69921875" customWidth="1"/>
-    <col min="11" max="11" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="64.09765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.59765625"/>
+    <col min="2" max="2" customWidth="true" width="26.59765625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.09765625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.8984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.59765625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.8984375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.69921875"/>
+    <col min="9" max="10" customWidth="true" width="12.69921875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.19921875"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.09765625"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.69921875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="64.09765625"/>
+    <col min="16" max="16" customWidth="true" width="7.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -567,47 +580,47 @@
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>9600809646</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>102</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="0">
         <v>600029</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="0">
         <v>111</v>
       </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="P2" t="s">
-        <v>27</v>
+      <c r="P2" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>